<commit_message>
dashboard overall stats done
</commit_message>
<xml_diff>
--- a/Final/amcharts generator.xlsx
+++ b/Final/amcharts generator.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yingxuan/Documents/SUTD/Term 5/ESA/Project/Viz-Wiz/Final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D12D44AF-3332-C047-896C-3F5050D7DF20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6A1AA7-2BB0-6F42-AA9F-21152F54C9C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46280" yWindow="2240" windowWidth="26840" windowHeight="15940" xr2:uid="{FF9CE252-0574-6F40-9EED-0D89605F4E5F}"/>
+    <workbookView xWindow="45160" yWindow="2240" windowWidth="26840" windowHeight="15940" xr2:uid="{FF9CE252-0574-6F40-9EED-0D89605F4E5F}"/>
   </bookViews>
   <sheets>
     <sheet name="formula" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -430,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBAA32D0-6842-7C46-9DC3-430ABA8AB6AE}">
-  <dimension ref="A1:F202"/>
+  <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A282" workbookViewId="0">
+      <selection activeCell="A299" sqref="A200:A299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -467,7 +467,7 @@
     <row r="2" spans="1:6">
       <c r="A2">
         <f ca="1">RANDBETWEEN(3,  80)</f>
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -485,7 +485,7 @@
     <row r="3" spans="1:6">
       <c r="A3">
         <f t="shared" ref="A3:A49" ca="1" si="0">RANDBETWEEN(3,  80)</f>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -503,7 +503,7 @@
     <row r="4" spans="1:6">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -521,7 +521,7 @@
     <row r="5" spans="1:6">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -539,7 +539,7 @@
     <row r="6" spans="1:6">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -557,7 +557,7 @@
     <row r="7" spans="1:6">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -575,7 +575,7 @@
     <row r="8" spans="1:6">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -593,7 +593,7 @@
     <row r="9" spans="1:6">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -611,7 +611,7 @@
     <row r="10" spans="1:6">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -629,7 +629,7 @@
     <row r="11" spans="1:6">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -647,7 +647,7 @@
     <row r="12" spans="1:6">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>75</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -665,7 +665,7 @@
     <row r="13" spans="1:6">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -683,7 +683,7 @@
     <row r="14" spans="1:6">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -701,7 +701,7 @@
     <row r="15" spans="1:6">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -719,7 +719,7 @@
     <row r="16" spans="1:6">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -737,7 +737,7 @@
     <row r="17" spans="1:6">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -755,7 +755,7 @@
     <row r="18" spans="1:6">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -773,7 +773,7 @@
     <row r="19" spans="1:6">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -791,7 +791,7 @@
     <row r="20" spans="1:6">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
@@ -809,7 +809,7 @@
     <row r="21" spans="1:6">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -827,7 +827,7 @@
     <row r="22" spans="1:6">
       <c r="A22">
         <f t="shared" ca="1" si="0"/>
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -845,7 +845,7 @@
     <row r="23" spans="1:6">
       <c r="A23">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -863,7 +863,7 @@
     <row r="24" spans="1:6">
       <c r="A24">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -881,7 +881,7 @@
     <row r="25" spans="1:6">
       <c r="A25">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -899,7 +899,7 @@
     <row r="26" spans="1:6">
       <c r="A26">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
@@ -917,7 +917,7 @@
     <row r="27" spans="1:6">
       <c r="A27">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -935,7 +935,7 @@
     <row r="28" spans="1:6">
       <c r="A28">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -953,7 +953,7 @@
     <row r="29" spans="1:6">
       <c r="A29">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -971,7 +971,7 @@
     <row r="30" spans="1:6">
       <c r="A30">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -989,7 +989,7 @@
     <row r="31" spans="1:6">
       <c r="A31">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -1007,7 +1007,7 @@
     <row r="32" spans="1:6">
       <c r="A32">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -1025,7 +1025,7 @@
     <row r="33" spans="1:6">
       <c r="A33">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -1043,7 +1043,7 @@
     <row r="34" spans="1:6">
       <c r="A34">
         <f ca="1">RANDBETWEEN(3,  80)</f>
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -1061,7 +1061,7 @@
     <row r="35" spans="1:6">
       <c r="A35">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -1079,7 +1079,7 @@
     <row r="36" spans="1:6">
       <c r="A36">
         <f t="shared" ca="1" si="0"/>
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -1097,7 +1097,7 @@
     <row r="37" spans="1:6">
       <c r="A37">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -1115,7 +1115,7 @@
     <row r="38" spans="1:6">
       <c r="A38">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -1133,7 +1133,7 @@
     <row r="39" spans="1:6">
       <c r="A39">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -1151,7 +1151,7 @@
     <row r="40" spans="1:6">
       <c r="A40">
         <f ca="1">RANDBETWEEN(3,  80)</f>
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1169,7 +1169,7 @@
     <row r="41" spans="1:6">
       <c r="A41">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -1187,7 +1187,7 @@
     <row r="42" spans="1:6">
       <c r="A42">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -1205,7 +1205,7 @@
     <row r="43" spans="1:6">
       <c r="A43">
         <f t="shared" ca="1" si="0"/>
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1223,7 +1223,7 @@
     <row r="44" spans="1:6">
       <c r="A44">
         <f t="shared" ca="1" si="0"/>
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -1241,7 +1241,7 @@
     <row r="45" spans="1:6">
       <c r="A45">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
@@ -1259,7 +1259,7 @@
     <row r="46" spans="1:6">
       <c r="A46">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -1277,7 +1277,7 @@
     <row r="47" spans="1:6">
       <c r="A47">
         <f t="shared" ca="1" si="0"/>
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
@@ -1295,7 +1295,7 @@
     <row r="48" spans="1:6">
       <c r="A48">
         <f t="shared" ca="1" si="0"/>
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -1313,7 +1313,7 @@
     <row r="49" spans="1:6">
       <c r="A49">
         <f t="shared" ca="1" si="0"/>
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -1331,7 +1331,7 @@
     <row r="50" spans="1:6">
       <c r="A50">
         <f ca="1">RANDBETWEEN(5, 20)</f>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -1349,7 +1349,7 @@
     <row r="51" spans="1:6">
       <c r="A51">
         <f t="shared" ref="A51:A70" ca="1" si="1">RANDBETWEEN(5, 20)</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -1367,7 +1367,7 @@
     <row r="52" spans="1:6">
       <c r="A52">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
@@ -1385,7 +1385,7 @@
     <row r="53" spans="1:6">
       <c r="A53">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
@@ -1403,7 +1403,7 @@
     <row r="54" spans="1:6">
       <c r="A54">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -1421,7 +1421,7 @@
     <row r="55" spans="1:6">
       <c r="A55">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
@@ -1439,7 +1439,7 @@
     <row r="56" spans="1:6">
       <c r="A56">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
@@ -1457,7 +1457,7 @@
     <row r="57" spans="1:6">
       <c r="A57">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
@@ -1475,7 +1475,7 @@
     <row r="58" spans="1:6">
       <c r="A58">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
@@ -1493,7 +1493,7 @@
     <row r="59" spans="1:6">
       <c r="A59">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C59" t="s">
         <v>7</v>
@@ -1511,7 +1511,7 @@
     <row r="60" spans="1:6">
       <c r="A60">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
         <v>7</v>
@@ -1529,7 +1529,7 @@
     <row r="61" spans="1:6">
       <c r="A61">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C61" t="s">
         <v>7</v>
@@ -1547,7 +1547,7 @@
     <row r="62" spans="1:6">
       <c r="A62">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
         <v>7</v>
@@ -1565,7 +1565,7 @@
     <row r="63" spans="1:6">
       <c r="A63">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C63" t="s">
         <v>7</v>
@@ -1583,7 +1583,7 @@
     <row r="64" spans="1:6">
       <c r="A64">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C64" t="s">
         <v>7</v>
@@ -1601,7 +1601,7 @@
     <row r="65" spans="1:6">
       <c r="A65">
         <f t="shared" ca="1" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
         <v>7</v>
@@ -1619,7 +1619,7 @@
     <row r="66" spans="1:6">
       <c r="A66">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
         <v>7</v>
@@ -1637,7 +1637,7 @@
     <row r="67" spans="1:6">
       <c r="A67">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C67" t="s">
         <v>7</v>
@@ -1655,7 +1655,7 @@
     <row r="68" spans="1:6">
       <c r="A68">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C68" t="s">
         <v>7</v>
@@ -1673,7 +1673,7 @@
     <row r="69" spans="1:6">
       <c r="A69">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C69" t="s">
         <v>7</v>
@@ -1691,7 +1691,7 @@
     <row r="70" spans="1:6">
       <c r="A70">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C70" t="s">
         <v>7</v>
@@ -1709,7 +1709,7 @@
     <row r="71" spans="1:6">
       <c r="A71">
         <f ca="1">RANDBETWEEN(5, 25)</f>
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C71" t="s">
         <v>7</v>
@@ -1727,7 +1727,7 @@
     <row r="72" spans="1:6">
       <c r="A72">
         <f t="shared" ref="A72:A100" ca="1" si="2">RANDBETWEEN(5, 25)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C72" t="s">
         <v>7</v>
@@ -1745,7 +1745,7 @@
     <row r="73" spans="1:6">
       <c r="A73">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C73" t="s">
         <v>7</v>
@@ -1763,7 +1763,7 @@
     <row r="74" spans="1:6">
       <c r="A74">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C74" t="s">
         <v>7</v>
@@ -1781,7 +1781,7 @@
     <row r="75" spans="1:6">
       <c r="A75">
         <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C75" t="s">
         <v>7</v>
@@ -1799,7 +1799,7 @@
     <row r="76" spans="1:6">
       <c r="A76">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C76" t="s">
         <v>7</v>
@@ -1817,7 +1817,7 @@
     <row r="77" spans="1:6">
       <c r="A77">
         <f t="shared" ca="1" si="2"/>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
@@ -1835,7 +1835,7 @@
     <row r="78" spans="1:6">
       <c r="A78">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C78" t="s">
         <v>6</v>
@@ -1853,7 +1853,7 @@
     <row r="79" spans="1:6">
       <c r="A79">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C79" t="s">
         <v>6</v>
@@ -1871,7 +1871,7 @@
     <row r="80" spans="1:6">
       <c r="A80">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
@@ -1889,7 +1889,7 @@
     <row r="81" spans="1:6">
       <c r="A81">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
@@ -1907,7 +1907,7 @@
     <row r="82" spans="1:6">
       <c r="A82">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
@@ -1925,7 +1925,7 @@
     <row r="83" spans="1:6">
       <c r="A83">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
@@ -1943,7 +1943,7 @@
     <row r="84" spans="1:6">
       <c r="A84">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -1961,7 +1961,7 @@
     <row r="85" spans="1:6">
       <c r="A85">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C85" t="s">
         <v>7</v>
@@ -1979,7 +1979,7 @@
     <row r="86" spans="1:6">
       <c r="A86">
         <f ca="1">RANDBETWEEN(5, 25)</f>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C86" t="s">
         <v>7</v>
@@ -1997,7 +1997,7 @@
     <row r="87" spans="1:6">
       <c r="A87">
         <f t="shared" ca="1" si="2"/>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C87" t="s">
         <v>7</v>
@@ -2015,7 +2015,7 @@
     <row r="88" spans="1:6">
       <c r="A88">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C88" t="s">
         <v>7</v>
@@ -2033,7 +2033,7 @@
     <row r="89" spans="1:6">
       <c r="A89">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C89" t="s">
         <v>7</v>
@@ -2051,7 +2051,7 @@
     <row r="90" spans="1:6">
       <c r="A90">
         <f t="shared" ca="1" si="2"/>
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C90" t="s">
         <v>7</v>
@@ -2069,7 +2069,7 @@
     <row r="91" spans="1:6">
       <c r="A91">
         <f t="shared" ca="1" si="2"/>
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
@@ -2087,7 +2087,7 @@
     <row r="92" spans="1:6">
       <c r="A92">
         <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C92" t="s">
         <v>7</v>
@@ -2105,7 +2105,7 @@
     <row r="93" spans="1:6">
       <c r="A93">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C93" t="s">
         <v>7</v>
@@ -2123,7 +2123,7 @@
     <row r="94" spans="1:6">
       <c r="A94">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C94" t="s">
         <v>7</v>
@@ -2141,7 +2141,7 @@
     <row r="95" spans="1:6">
       <c r="A95">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C95" t="s">
         <v>7</v>
@@ -2159,7 +2159,7 @@
     <row r="96" spans="1:6">
       <c r="A96">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C96" t="s">
         <v>7</v>
@@ -2177,7 +2177,7 @@
     <row r="97" spans="1:6">
       <c r="A97">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C97" t="s">
         <v>7</v>
@@ -2195,7 +2195,7 @@
     <row r="98" spans="1:6">
       <c r="A98">
         <f t="shared" ca="1" si="2"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
@@ -2213,7 +2213,7 @@
     <row r="99" spans="1:6">
       <c r="A99">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C99" t="s">
         <v>7</v>
@@ -2231,7 +2231,7 @@
     <row r="100" spans="1:6">
       <c r="A100">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="C100" t="s">
         <v>7</v>
@@ -2249,7 +2249,7 @@
     <row r="101" spans="1:6">
       <c r="A101">
         <f ca="1">RANDBETWEEN(3,  80)</f>
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="C101" t="s">
         <v>7</v>
@@ -2267,7 +2267,7 @@
     <row r="102" spans="1:6">
       <c r="A102">
         <f t="shared" ref="A102:A148" ca="1" si="3">RANDBETWEEN(3,  80)</f>
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="C102" t="s">
         <v>6</v>
@@ -2285,7 +2285,7 @@
     <row r="103" spans="1:6">
       <c r="A103">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C103" t="s">
         <v>6</v>
@@ -2303,7 +2303,7 @@
     <row r="104" spans="1:6">
       <c r="A104">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
@@ -2321,7 +2321,7 @@
     <row r="105" spans="1:6">
       <c r="A105">
         <f t="shared" ca="1" si="3"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C105" t="s">
         <v>6</v>
@@ -2339,7 +2339,7 @@
     <row r="106" spans="1:6">
       <c r="A106">
         <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C106" t="s">
         <v>6</v>
@@ -2357,7 +2357,7 @@
     <row r="107" spans="1:6">
       <c r="A107">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="C107" t="s">
         <v>6</v>
@@ -2375,7 +2375,7 @@
     <row r="108" spans="1:6">
       <c r="A108">
         <f t="shared" ca="1" si="3"/>
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C108" t="s">
         <v>6</v>
@@ -2393,7 +2393,7 @@
     <row r="109" spans="1:6">
       <c r="A109">
         <f t="shared" ca="1" si="3"/>
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C109" t="s">
         <v>7</v>
@@ -2411,7 +2411,7 @@
     <row r="110" spans="1:6">
       <c r="A110">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="C110" t="s">
         <v>7</v>
@@ -2429,7 +2429,7 @@
     <row r="111" spans="1:6">
       <c r="A111">
         <f t="shared" ca="1" si="3"/>
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C111" t="s">
         <v>7</v>
@@ -2447,7 +2447,7 @@
     <row r="112" spans="1:6">
       <c r="A112">
         <f t="shared" ca="1" si="3"/>
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C112" t="s">
         <v>7</v>
@@ -2465,7 +2465,7 @@
     <row r="113" spans="1:6">
       <c r="A113">
         <f t="shared" ca="1" si="3"/>
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C113" t="s">
         <v>7</v>
@@ -2483,7 +2483,7 @@
     <row r="114" spans="1:6">
       <c r="A114">
         <f t="shared" ca="1" si="3"/>
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="C114" t="s">
         <v>7</v>
@@ -2501,7 +2501,7 @@
     <row r="115" spans="1:6">
       <c r="A115">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C115" t="s">
         <v>7</v>
@@ -2519,7 +2519,7 @@
     <row r="116" spans="1:6">
       <c r="A116">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="C116" t="s">
         <v>7</v>
@@ -2537,7 +2537,7 @@
     <row r="117" spans="1:6">
       <c r="A117">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C117" t="s">
         <v>7</v>
@@ -2555,7 +2555,7 @@
     <row r="118" spans="1:6">
       <c r="A118">
         <f t="shared" ca="1" si="3"/>
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C118" t="s">
         <v>7</v>
@@ -2573,7 +2573,7 @@
     <row r="119" spans="1:6">
       <c r="A119">
         <f t="shared" ca="1" si="3"/>
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="C119" t="s">
         <v>7</v>
@@ -2591,7 +2591,7 @@
     <row r="120" spans="1:6">
       <c r="A120">
         <f t="shared" ca="1" si="3"/>
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C120" t="s">
         <v>7</v>
@@ -2609,7 +2609,7 @@
     <row r="121" spans="1:6">
       <c r="A121">
         <f t="shared" ca="1" si="3"/>
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="C121" t="s">
         <v>7</v>
@@ -2627,7 +2627,7 @@
     <row r="122" spans="1:6">
       <c r="A122">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C122" t="s">
         <v>7</v>
@@ -2645,7 +2645,7 @@
     <row r="123" spans="1:6">
       <c r="A123">
         <f t="shared" ca="1" si="3"/>
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C123" t="s">
         <v>6</v>
@@ -2663,7 +2663,7 @@
     <row r="124" spans="1:6">
       <c r="A124">
         <f t="shared" ca="1" si="3"/>
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="C124" t="s">
         <v>6</v>
@@ -2681,7 +2681,7 @@
     <row r="125" spans="1:6">
       <c r="A125">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="C125" t="s">
         <v>6</v>
@@ -2699,7 +2699,7 @@
     <row r="126" spans="1:6">
       <c r="A126">
         <f t="shared" ca="1" si="3"/>
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C126" t="s">
         <v>6</v>
@@ -2717,7 +2717,7 @@
     <row r="127" spans="1:6">
       <c r="A127">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C127" t="s">
         <v>6</v>
@@ -2735,7 +2735,7 @@
     <row r="128" spans="1:6">
       <c r="A128">
         <f t="shared" ca="1" si="3"/>
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="C128" t="s">
         <v>6</v>
@@ -2753,7 +2753,7 @@
     <row r="129" spans="1:6">
       <c r="A129">
         <f t="shared" ca="1" si="3"/>
-        <v>57</v>
+        <v>15</v>
       </c>
       <c r="C129" t="s">
         <v>6</v>
@@ -2771,7 +2771,7 @@
     <row r="130" spans="1:6">
       <c r="A130">
         <f t="shared" ca="1" si="3"/>
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C130" t="s">
         <v>7</v>
@@ -2789,7 +2789,7 @@
     <row r="131" spans="1:6">
       <c r="A131">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="C131" t="s">
         <v>7</v>
@@ -2807,7 +2807,7 @@
     <row r="132" spans="1:6">
       <c r="A132">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C132" t="s">
         <v>7</v>
@@ -2825,7 +2825,7 @@
     <row r="133" spans="1:6">
       <c r="A133">
         <f ca="1">RANDBETWEEN(3,  80)</f>
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C133" t="s">
         <v>7</v>
@@ -2843,7 +2843,7 @@
     <row r="134" spans="1:6">
       <c r="A134">
         <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>62</v>
       </c>
       <c r="C134" t="s">
         <v>7</v>
@@ -2861,7 +2861,7 @@
     <row r="135" spans="1:6">
       <c r="A135">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C135" t="s">
         <v>7</v>
@@ -2879,7 +2879,7 @@
     <row r="136" spans="1:6">
       <c r="A136">
         <f t="shared" ca="1" si="3"/>
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C136" t="s">
         <v>7</v>
@@ -2897,7 +2897,7 @@
     <row r="137" spans="1:6">
       <c r="A137">
         <f t="shared" ca="1" si="3"/>
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C137" t="s">
         <v>7</v>
@@ -2915,7 +2915,7 @@
     <row r="138" spans="1:6">
       <c r="A138">
         <f t="shared" ca="1" si="3"/>
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C138" t="s">
         <v>7</v>
@@ -2933,7 +2933,7 @@
     <row r="139" spans="1:6">
       <c r="A139">
         <f ca="1">RANDBETWEEN(3,  80)</f>
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C139" t="s">
         <v>7</v>
@@ -2951,7 +2951,7 @@
     <row r="140" spans="1:6">
       <c r="A140">
         <f t="shared" ca="1" si="3"/>
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C140" t="s">
         <v>7</v>
@@ -2969,7 +2969,7 @@
     <row r="141" spans="1:6">
       <c r="A141">
         <f t="shared" ca="1" si="3"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C141" t="s">
         <v>7</v>
@@ -2987,7 +2987,7 @@
     <row r="142" spans="1:6">
       <c r="A142">
         <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C142" t="s">
         <v>7</v>
@@ -3005,7 +3005,7 @@
     <row r="143" spans="1:6">
       <c r="A143">
         <f t="shared" ca="1" si="3"/>
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="C143" t="s">
         <v>7</v>
@@ -3023,7 +3023,7 @@
     <row r="144" spans="1:6">
       <c r="A144">
         <f t="shared" ca="1" si="3"/>
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C144" t="s">
         <v>7</v>
@@ -3041,7 +3041,7 @@
     <row r="145" spans="1:6">
       <c r="A145">
         <f t="shared" ca="1" si="3"/>
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C145" t="s">
         <v>7</v>
@@ -3059,7 +3059,7 @@
     <row r="146" spans="1:6">
       <c r="A146">
         <f t="shared" ca="1" si="3"/>
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
@@ -3077,7 +3077,7 @@
     <row r="147" spans="1:6">
       <c r="A147">
         <f t="shared" ca="1" si="3"/>
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C147" t="s">
         <v>6</v>
@@ -3095,7 +3095,7 @@
     <row r="148" spans="1:6">
       <c r="A148">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="C148" t="s">
         <v>6</v>
@@ -3113,7 +3113,7 @@
     <row r="149" spans="1:6">
       <c r="A149">
         <f ca="1">RANDBETWEEN(5, 20)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C149" t="s">
         <v>6</v>
@@ -3131,7 +3131,7 @@
     <row r="150" spans="1:6">
       <c r="A150">
         <f t="shared" ref="A150:A169" ca="1" si="4">RANDBETWEEN(5, 20)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C150" t="s">
         <v>6</v>
@@ -3149,7 +3149,7 @@
     <row r="151" spans="1:6">
       <c r="A151">
         <f t="shared" ca="1" si="4"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C151" t="s">
         <v>6</v>
@@ -3167,7 +3167,7 @@
     <row r="152" spans="1:6">
       <c r="A152">
         <f t="shared" ca="1" si="4"/>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="C152" t="s">
         <v>6</v>
@@ -3185,7 +3185,7 @@
     <row r="153" spans="1:6">
       <c r="A153">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C153" t="s">
         <v>7</v>
@@ -3203,7 +3203,7 @@
     <row r="154" spans="1:6">
       <c r="A154">
         <f t="shared" ca="1" si="4"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C154" t="s">
         <v>7</v>
@@ -3221,7 +3221,7 @@
     <row r="155" spans="1:6">
       <c r="A155">
         <f t="shared" ca="1" si="4"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C155" t="s">
         <v>7</v>
@@ -3257,7 +3257,7 @@
     <row r="157" spans="1:6">
       <c r="A157">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C157" t="s">
         <v>7</v>
@@ -3275,7 +3275,7 @@
     <row r="158" spans="1:6">
       <c r="A158">
         <f t="shared" ca="1" si="4"/>
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C158" t="s">
         <v>7</v>
@@ -3293,7 +3293,7 @@
     <row r="159" spans="1:6">
       <c r="A159">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C159" t="s">
         <v>7</v>
@@ -3311,7 +3311,7 @@
     <row r="160" spans="1:6">
       <c r="A160">
         <f t="shared" ca="1" si="4"/>
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C160" t="s">
         <v>7</v>
@@ -3329,7 +3329,7 @@
     <row r="161" spans="1:6">
       <c r="A161">
         <f t="shared" ca="1" si="4"/>
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C161" t="s">
         <v>7</v>
@@ -3347,7 +3347,7 @@
     <row r="162" spans="1:6">
       <c r="A162">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C162" t="s">
         <v>7</v>
@@ -3365,7 +3365,7 @@
     <row r="163" spans="1:6">
       <c r="A163">
         <f t="shared" ca="1" si="4"/>
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C163" t="s">
         <v>7</v>
@@ -3383,7 +3383,7 @@
     <row r="164" spans="1:6">
       <c r="A164">
         <f t="shared" ca="1" si="4"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C164" t="s">
         <v>7</v>
@@ -3401,7 +3401,7 @@
     <row r="165" spans="1:6">
       <c r="A165">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C165" t="s">
         <v>7</v>
@@ -3419,7 +3419,7 @@
     <row r="166" spans="1:6">
       <c r="A166">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C166" t="s">
         <v>7</v>
@@ -3437,7 +3437,7 @@
     <row r="167" spans="1:6">
       <c r="A167">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C167" t="s">
         <v>7</v>
@@ -3455,7 +3455,7 @@
     <row r="168" spans="1:6">
       <c r="A168">
         <f t="shared" ca="1" si="4"/>
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C168" t="s">
         <v>7</v>
@@ -3473,7 +3473,7 @@
     <row r="169" spans="1:6">
       <c r="A169">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C169" t="s">
         <v>6</v>
@@ -3491,7 +3491,7 @@
     <row r="170" spans="1:6">
       <c r="A170">
         <f ca="1">RANDBETWEEN(5, 25)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C170" t="s">
         <v>6</v>
@@ -3508,8 +3508,8 @@
     </row>
     <row r="171" spans="1:6">
       <c r="A171">
-        <f t="shared" ref="A171:A199" ca="1" si="5">RANDBETWEEN(5, 25)</f>
-        <v>8</v>
+        <f t="shared" ref="A171:A234" ca="1" si="5">RANDBETWEEN(5, 25)</f>
+        <v>5</v>
       </c>
       <c r="C171" t="s">
         <v>6</v>
@@ -3527,7 +3527,7 @@
     <row r="172" spans="1:6">
       <c r="A172">
         <f t="shared" ca="1" si="5"/>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C172" t="s">
         <v>6</v>
@@ -3545,7 +3545,7 @@
     <row r="173" spans="1:6">
       <c r="A173">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C173" t="s">
         <v>6</v>
@@ -3563,7 +3563,7 @@
     <row r="174" spans="1:6">
       <c r="A174">
         <f t="shared" ca="1" si="5"/>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C174" t="s">
         <v>6</v>
@@ -3581,7 +3581,7 @@
     <row r="175" spans="1:6">
       <c r="A175">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="C175" t="s">
         <v>6</v>
@@ -3599,7 +3599,7 @@
     <row r="176" spans="1:6">
       <c r="A176">
         <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C176" t="s">
         <v>7</v>
@@ -3617,7 +3617,7 @@
     <row r="177" spans="1:6">
       <c r="A177">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C177" t="s">
         <v>7</v>
@@ -3635,7 +3635,7 @@
     <row r="178" spans="1:6">
       <c r="A178">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C178" t="s">
         <v>7</v>
@@ -3653,7 +3653,7 @@
     <row r="179" spans="1:6">
       <c r="A179">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C179" t="s">
         <v>7</v>
@@ -3671,7 +3671,7 @@
     <row r="180" spans="1:6">
       <c r="A180">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C180" t="s">
         <v>7</v>
@@ -3689,7 +3689,7 @@
     <row r="181" spans="1:6">
       <c r="A181">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C181" t="s">
         <v>7</v>
@@ -3707,7 +3707,7 @@
     <row r="182" spans="1:6">
       <c r="A182">
         <f t="shared" ca="1" si="5"/>
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C182" t="s">
         <v>7</v>
@@ -3725,7 +3725,7 @@
     <row r="183" spans="1:6">
       <c r="A183">
         <f t="shared" ca="1" si="5"/>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C183" t="s">
         <v>7</v>
@@ -3743,7 +3743,7 @@
     <row r="184" spans="1:6">
       <c r="A184">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C184" t="s">
         <v>7</v>
@@ -3761,7 +3761,7 @@
     <row r="185" spans="1:6">
       <c r="A185">
         <f ca="1">RANDBETWEEN(5, 25)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C185" t="s">
         <v>7</v>
@@ -3779,7 +3779,7 @@
     <row r="186" spans="1:6">
       <c r="A186">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C186" t="s">
         <v>7</v>
@@ -3797,7 +3797,7 @@
     <row r="187" spans="1:6">
       <c r="A187">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C187" t="s">
         <v>7</v>
@@ -3815,7 +3815,7 @@
     <row r="188" spans="1:6">
       <c r="A188">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C188" t="s">
         <v>7</v>
@@ -3851,7 +3851,7 @@
     <row r="190" spans="1:6">
       <c r="A190">
         <f t="shared" ca="1" si="5"/>
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C190" t="s">
         <v>6</v>
@@ -3869,7 +3869,7 @@
     <row r="191" spans="1:6">
       <c r="A191">
         <f t="shared" ca="1" si="5"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C191" t="s">
         <v>6</v>
@@ -3887,7 +3887,7 @@
     <row r="192" spans="1:6">
       <c r="A192">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C192" t="s">
         <v>6</v>
@@ -3905,7 +3905,7 @@
     <row r="193" spans="1:6">
       <c r="A193">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C193" t="s">
         <v>6</v>
@@ -3923,7 +3923,7 @@
     <row r="194" spans="1:6">
       <c r="A194">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C194" t="s">
         <v>6</v>
@@ -3941,7 +3941,7 @@
     <row r="195" spans="1:6">
       <c r="A195">
         <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C195" t="s">
         <v>6</v>
@@ -3959,7 +3959,7 @@
     <row r="196" spans="1:6">
       <c r="A196">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C196" t="s">
         <v>6</v>
@@ -3977,7 +3977,7 @@
     <row r="197" spans="1:6">
       <c r="A197">
         <f t="shared" ca="1" si="5"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C197" t="s">
         <v>7</v>
@@ -3995,7 +3995,7 @@
     <row r="198" spans="1:6">
       <c r="A198">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C198" t="s">
         <v>7</v>
@@ -4013,7 +4013,7 @@
     <row r="199" spans="1:6">
       <c r="A199">
         <f t="shared" ca="1" si="5"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C199" t="s">
         <v>7</v>
@@ -4029,16 +4029,610 @@
       </c>
     </row>
     <row r="200" spans="1:6">
+      <c r="A200">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
       <c r="E200" s="2"/>
       <c r="F200" s="2"/>
     </row>
     <row r="201" spans="1:6">
+      <c r="A201">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
       <c r="E201" s="2"/>
       <c r="F201" s="2"/>
     </row>
     <row r="202" spans="1:6">
+      <c r="A202">
+        <f t="shared" ca="1" si="5"/>
+        <v>22</v>
+      </c>
       <c r="E202" s="2"/>
       <c r="F202" s="2"/>
+    </row>
+    <row r="203" spans="1:6">
+      <c r="A203">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204">
+        <f t="shared" ca="1" si="5"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205">
+        <f t="shared" ca="1" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
+      <c r="A207">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
+      <c r="A208">
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210">
+        <f t="shared" ca="1" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211">
+        <f t="shared" ca="1" si="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212">
+        <f t="shared" ca="1" si="5"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215">
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216">
+        <f t="shared" ca="1" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218">
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219">
+        <f t="shared" ca="1" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220">
+        <f t="shared" ca="1" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221">
+        <f t="shared" ca="1" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222">
+        <f t="shared" ca="1" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223">
+        <f t="shared" ca="1" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224">
+        <f t="shared" ca="1" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225">
+        <f t="shared" ca="1" si="5"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226">
+        <f t="shared" ca="1" si="5"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227">
+        <f t="shared" ca="1" si="5"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228">
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229">
+        <f t="shared" ca="1" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230">
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231">
+        <f t="shared" ca="1" si="5"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232">
+        <f t="shared" ca="1" si="5"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233">
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234">
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235">
+        <f ca="1">RANDBETWEEN(3, 80)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236">
+        <f t="shared" ref="A236:A299" ca="1" si="6">RANDBETWEEN(3, 80)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237">
+        <f t="shared" ca="1" si="6"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238">
+        <f t="shared" ca="1" si="6"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239">
+        <f t="shared" ca="1" si="6"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240">
+        <f t="shared" ca="1" si="6"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241">
+        <f t="shared" ca="1" si="6"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242">
+        <f t="shared" ca="1" si="6"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243">
+        <f t="shared" ca="1" si="6"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244">
+        <f t="shared" ca="1" si="6"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245">
+        <f t="shared" ca="1" si="6"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246">
+        <f t="shared" ca="1" si="6"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247">
+        <f t="shared" ca="1" si="6"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248">
+        <f t="shared" ca="1" si="6"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249">
+        <f t="shared" ca="1" si="6"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250">
+        <f t="shared" ca="1" si="6"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251">
+        <f t="shared" ca="1" si="6"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252">
+        <f t="shared" ca="1" si="6"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253">
+        <f t="shared" ca="1" si="6"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254">
+        <f t="shared" ca="1" si="6"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255">
+        <f t="shared" ca="1" si="6"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256">
+        <f t="shared" ca="1" si="6"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257">
+        <f t="shared" ca="1" si="6"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258">
+        <f t="shared" ca="1" si="6"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259">
+        <f t="shared" ca="1" si="6"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260">
+        <f t="shared" ca="1" si="6"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261">
+        <f t="shared" ca="1" si="6"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262">
+        <f t="shared" ca="1" si="6"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263">
+        <f t="shared" ca="1" si="6"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264">
+        <f t="shared" ca="1" si="6"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265">
+        <f t="shared" ca="1" si="6"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266">
+        <f t="shared" ca="1" si="6"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1">
+      <c r="A267">
+        <f t="shared" ca="1" si="6"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1">
+      <c r="A268">
+        <f t="shared" ca="1" si="6"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1">
+      <c r="A269">
+        <f t="shared" ca="1" si="6"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1">
+      <c r="A270">
+        <f t="shared" ca="1" si="6"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1">
+      <c r="A271">
+        <f t="shared" ca="1" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1">
+      <c r="A272">
+        <f t="shared" ca="1" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1">
+      <c r="A273">
+        <f t="shared" ca="1" si="6"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1">
+      <c r="A274">
+        <f t="shared" ca="1" si="6"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1">
+      <c r="A275">
+        <f t="shared" ca="1" si="6"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1">
+      <c r="A276">
+        <f t="shared" ca="1" si="6"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1">
+      <c r="A277">
+        <f t="shared" ca="1" si="6"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1">
+      <c r="A278">
+        <f t="shared" ca="1" si="6"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279">
+        <f t="shared" ca="1" si="6"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1">
+      <c r="A280">
+        <f t="shared" ca="1" si="6"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1">
+      <c r="A281">
+        <f t="shared" ca="1" si="6"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1">
+      <c r="A282">
+        <f t="shared" ca="1" si="6"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1">
+      <c r="A283">
+        <f t="shared" ca="1" si="6"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1">
+      <c r="A284">
+        <f t="shared" ca="1" si="6"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1">
+      <c r="A285">
+        <f t="shared" ca="1" si="6"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1">
+      <c r="A286">
+        <f t="shared" ca="1" si="6"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1">
+      <c r="A287">
+        <f t="shared" ca="1" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1">
+      <c r="A288">
+        <f t="shared" ca="1" si="6"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1">
+      <c r="A289">
+        <f t="shared" ca="1" si="6"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1">
+      <c r="A290">
+        <f t="shared" ca="1" si="6"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1">
+      <c r="A291">
+        <f t="shared" ca="1" si="6"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1">
+      <c r="A292">
+        <f t="shared" ca="1" si="6"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1">
+      <c r="A293">
+        <f t="shared" ca="1" si="6"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1">
+      <c r="A294">
+        <f t="shared" ca="1" si="6"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1">
+      <c r="A295">
+        <f t="shared" ca="1" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1">
+      <c r="A296">
+        <f t="shared" ca="1" si="6"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1">
+      <c r="A297">
+        <f t="shared" ca="1" si="6"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1">
+      <c r="A298">
+        <f t="shared" ca="1" si="6"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1">
+      <c r="A299">
+        <f t="shared" ca="1" si="6"/>
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>